<commit_message>
new: added west-gate file parsing
</commit_message>
<xml_diff>
--- a/src/files/meta/xml-list/xml_list.xlsx
+++ b/src/files/meta/xml-list/xml_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kitchen-time\crawler\src\files\meta\xml-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFE7ADE8-A21D-44A4-A0B7-C8928668177D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B8C967-08FA-4F29-8388-7E02D84FE76F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD070FBF-2C98-4468-8316-301635C9CAD9}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
   <si>
     <t>Поставщик</t>
   </si>
@@ -45,36 +44,9 @@
     <t>Бренд</t>
   </si>
   <si>
-    <t>Анна Лафарг</t>
-  </si>
-  <si>
-    <t>https://www.fissler-shop.ru/u/annalafarg.xml</t>
-  </si>
-  <si>
     <t>xml</t>
   </si>
   <si>
-    <t>ANNA LAFARG</t>
-  </si>
-  <si>
-    <t>CONTINENTA</t>
-  </si>
-  <si>
-    <t>EASY LIFE</t>
-  </si>
-  <si>
-    <t>FISSLER</t>
-  </si>
-  <si>
-    <t>JULIA VYSOTSKAYA</t>
-  </si>
-  <si>
-    <t>LEGNOART</t>
-  </si>
-  <si>
-    <t>MAXWELL &amp; WILLIAMS</t>
-  </si>
-  <si>
     <t>Лимарс</t>
   </si>
   <si>
@@ -226,6 +198,42 @@
   </si>
   <si>
     <t>STAUB</t>
+  </si>
+  <si>
+    <t>West Gate</t>
+  </si>
+  <si>
+    <t>https://west-gate.ru/yml.xml</t>
+  </si>
+  <si>
+    <t>PACOJET</t>
+  </si>
+  <si>
+    <t>POLYSCIENCE</t>
+  </si>
+  <si>
+    <t>SOUSVIDETOOLS</t>
+  </si>
+  <si>
+    <t>FRUCOSOL</t>
+  </si>
+  <si>
+    <t>WARING LAB</t>
+  </si>
+  <si>
+    <t>CENTURION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELOMA </t>
+  </si>
+  <si>
+    <t>WVT</t>
+  </si>
+  <si>
+    <t>WARING</t>
+  </si>
+  <si>
+    <t>HOTMIX</t>
   </si>
 </sst>
 </file>
@@ -693,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CAE84D-4C01-4439-95AA-D773DDD0058D}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -724,471 +732,501 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>6</v>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>21</v>
+      <c r="C12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="6" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="12" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="9" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="6" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="9" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="6" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="B30" s="12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="C30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="9" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="C31" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="6" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="B32" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="C32" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="12" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="9" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="5" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="6" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="12" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="9" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="6" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="9" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="9" t="s">
+      <c r="C43" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="6" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="9" t="s">
+      <c r="B44" s="12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="6" t="s">
+      <c r="C44" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="9" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="6" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="7"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="9" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{A9775152-7F3E-4348-AE6A-E1A8454A36FD}"/>
-    <hyperlink ref="B9" r:id="rId2" xr:uid="{62EB30E0-4666-46F2-BE87-1548C3ED9CD5}"/>
-    <hyperlink ref="B12" r:id="rId3" xr:uid="{E97AF6BB-2147-4552-B5B6-A1485FC73360}"/>
-    <hyperlink ref="B15" r:id="rId4" display="https://www.finedesigngroup.ru/bitrix/catalog_export/fine_f_yandex_vendor_export.php" xr:uid="{1A22A5C6-4106-4FFF-BA8C-ACAB8C4ED2FE}"/>
-    <hyperlink ref="B27" r:id="rId5" xr:uid="{16E48248-65E0-4C44-A361-B0C288D566FF}"/>
-    <hyperlink ref="B28" r:id="rId6" xr:uid="{13DE13FF-D4C7-45A2-99C0-4BCD5C0198D3}"/>
-    <hyperlink ref="B29" r:id="rId7" xr:uid="{8BE26B7F-2777-46F8-92FB-B3312B94F00C}"/>
-    <hyperlink ref="B40" r:id="rId8" xr:uid="{6305E34C-8789-45CE-AB83-0AB94999553A}"/>
-    <hyperlink ref="B41" r:id="rId9" xr:uid="{B3A45B41-73BA-4FF3-8FFE-B803B4B36956}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{62EB30E0-4666-46F2-BE87-1548C3ED9CD5}"/>
+    <hyperlink ref="B15" r:id="rId3" xr:uid="{E97AF6BB-2147-4552-B5B6-A1485FC73360}"/>
+    <hyperlink ref="B18" r:id="rId4" display="https://www.finedesigngroup.ru/bitrix/catalog_export/fine_f_yandex_vendor_export.php" xr:uid="{1A22A5C6-4106-4FFF-BA8C-ACAB8C4ED2FE}"/>
+    <hyperlink ref="B30" r:id="rId5" xr:uid="{16E48248-65E0-4C44-A361-B0C288D566FF}"/>
+    <hyperlink ref="B31" r:id="rId6" xr:uid="{13DE13FF-D4C7-45A2-99C0-4BCD5C0198D3}"/>
+    <hyperlink ref="B32" r:id="rId7" xr:uid="{8BE26B7F-2777-46F8-92FB-B3312B94F00C}"/>
+    <hyperlink ref="B43" r:id="rId8" xr:uid="{6305E34C-8789-45CE-AB83-0AB94999553A}"/>
+    <hyperlink ref="B44" r:id="rId9" xr:uid="{B3A45B41-73BA-4FF3-8FFE-B803B4B36956}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
old update, added AnnaLafarg
</commit_message>
<xml_diff>
--- a/src/files/meta/xml-list/xml_list.xlsx
+++ b/src/files/meta/xml-list/xml_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kitchen-time\crawler\src\files\meta\xml-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kitchen-time\crawler\src\files\meta\xml-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B8C967-08FA-4F29-8388-7E02D84FE76F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C002815-5FB9-4C39-A29E-04BEE2B53BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD070FBF-2C98-4468-8316-301635C9CAD9}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
   <si>
     <t>Поставщик</t>
   </si>
@@ -86,9 +87,6 @@
     <t>CIRCULON</t>
   </si>
   <si>
-    <t>EVA SOLO</t>
-  </si>
-  <si>
     <t>GUZZINI</t>
   </si>
   <si>
@@ -143,27 +141,15 @@
     <t>https://homefeel.ru/xml/export_blumica_partners.xml</t>
   </si>
   <si>
-    <t>ANDREA HOUSE</t>
-  </si>
-  <si>
-    <t>ARGENESI</t>
-  </si>
-  <si>
     <t>BASTION COLLECTIONS</t>
   </si>
   <si>
-    <t>BLOOMIX</t>
-  </si>
-  <si>
     <t>FADE</t>
   </si>
   <si>
     <t>IVV</t>
   </si>
   <si>
-    <t>KITCHEN CRAFT</t>
-  </si>
-  <si>
     <t>KOENITZ</t>
   </si>
   <si>
@@ -234,6 +220,45 @@
   </si>
   <si>
     <t>HOTMIX</t>
+  </si>
+  <si>
+    <t>COSY&amp;TRENDY</t>
+  </si>
+  <si>
+    <t>BISETTI</t>
+  </si>
+  <si>
+    <t>COMAS</t>
+  </si>
+  <si>
+    <t>ARIANE</t>
+  </si>
+  <si>
+    <t>ZWILLING</t>
+  </si>
+  <si>
+    <t>LIBERTY JONES</t>
+  </si>
+  <si>
+    <t>https://www.fissler-shop.ru/u/annalafarg.xml</t>
+  </si>
+  <si>
+    <t>EASY LIFE</t>
+  </si>
+  <si>
+    <t>FISSLER</t>
+  </si>
+  <si>
+    <t>JULIA VYSOTSKAYA</t>
+  </si>
+  <si>
+    <t>MAXWELL &amp; WILLIAMS</t>
+  </si>
+  <si>
+    <t>ANNA LAFARG</t>
+  </si>
+  <si>
+    <t>Anna Lafarg</t>
   </si>
 </sst>
 </file>
@@ -701,16 +726,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CAE84D-4C01-4439-95AA-D773DDD0058D}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" style="3" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="3"/>
@@ -732,16 +757,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -751,7 +776,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -761,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -771,7 +796,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -781,7 +806,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -791,7 +816,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -801,7 +826,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -811,7 +836,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -821,7 +846,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -831,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -917,92 +942,92 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="6" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1013,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1023,109 +1048,109 @@
         <v>4</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="C30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="C31" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>37</v>
+      <c r="A32" s="10"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>39</v>
+      <c r="A34" s="10"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="5"/>
+      <c r="C35" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
+      <c r="A36" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="C36" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>42</v>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>43</v>
+      <c r="A38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1135,7 +1160,7 @@
         <v>4</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1145,7 +1170,7 @@
         <v>4</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1155,7 +1180,7 @@
         <v>4</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1165,55 +1190,119 @@
         <v>4</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>54</v>
+      <c r="A45" s="7"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>55</v>
+      <c r="A46" s="10"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="7"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="7"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="7"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1224,9 +1313,10 @@
     <hyperlink ref="B18" r:id="rId4" display="https://www.finedesigngroup.ru/bitrix/catalog_export/fine_f_yandex_vendor_export.php" xr:uid="{1A22A5C6-4106-4FFF-BA8C-ACAB8C4ED2FE}"/>
     <hyperlink ref="B30" r:id="rId5" xr:uid="{16E48248-65E0-4C44-A361-B0C288D566FF}"/>
     <hyperlink ref="B31" r:id="rId6" xr:uid="{13DE13FF-D4C7-45A2-99C0-4BCD5C0198D3}"/>
-    <hyperlink ref="B32" r:id="rId7" xr:uid="{8BE26B7F-2777-46F8-92FB-B3312B94F00C}"/>
+    <hyperlink ref="B36" r:id="rId7" xr:uid="{8BE26B7F-2777-46F8-92FB-B3312B94F00C}"/>
     <hyperlink ref="B43" r:id="rId8" xr:uid="{6305E34C-8789-45CE-AB83-0AB94999553A}"/>
     <hyperlink ref="B44" r:id="rId9" xr:uid="{B3A45B41-73BA-4FF3-8FFE-B803B4B36956}"/>
+    <hyperlink ref="B48" r:id="rId10" xr:uid="{EF383C45-7C49-4331-B8B4-CD7A891F9240}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>